<commit_message>
Add text/date SQL intro and update scripts/slides
Added TEXT_DATE_INTRODUCTION script for SQL text and date functions. Removed Lec_0/Create_Table and added a placeholder Create_Table for the Credit Card project. Updated math_text_function_2 script to clean up date/time function examples. Updated slides Lec_3_4.xlsx and Lec_5_6.xlsx.
</commit_message>
<xml_diff>
--- a/Beginner/Slides/Lec_5_6.xlsx
+++ b/Beginner/Slides/Lec_5_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ABF119-DB0A-4542-893C-057688CA830A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FAB699-D250-3343-A5F2-98A9683EAF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="2" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="WHERE" sheetId="9" r:id="rId5"/>
     <sheet name="Date" sheetId="12" r:id="rId6"/>
     <sheet name="Group" sheetId="13" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Group!$A$1:$E$51</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="980">
   <si>
     <t>- 9年软件开发经验，擅长数据库、Python、AI</t>
   </si>
@@ -2893,6 +2894,321 @@
   </si>
   <si>
     <t>SELECT department_id, COUNT(student_id) AS student_count</t>
+  </si>
+  <si>
+    <t>1–10. 条件与逻辑运算（AND, OR, NOT, BETWEEN, IN, IS NULL）</t>
+  </si>
+  <si>
+    <t>查询GPA在3.0到4.0之间且年龄小于22岁的学生。</t>
+  </si>
+  <si>
+    <t>Find students whose GPA is between 3.0 and 4.0 and age is less than 22.</t>
+  </si>
+  <si>
+    <t>查找不是“男”性别，且不在1、2、3系的学生信息。</t>
+  </si>
+  <si>
+    <t>Find students who are not male and not in departments 1, 2, or 3.</t>
+  </si>
+  <si>
+    <t>查询选修了课程ID为1或3，但成绩低于60的学生ID。</t>
+  </si>
+  <si>
+    <t>Find student IDs who enrolled in course 1 or 3 and scored below 60.</t>
+  </si>
+  <si>
+    <t>查询出生年份不是2002或2003的学生。</t>
+  </si>
+  <si>
+    <t>Find students whose birth year is not 2002 or 2003.</t>
+  </si>
+  <si>
+    <t>查找教授中，工资在9000到11000之间，且不是2016年或2020年入职的。</t>
+  </si>
+  <si>
+    <t>Find professors whose salary is between 9000 and 11000 and were not hired in 2016 or 2020.</t>
+  </si>
+  <si>
+    <t>查询没有GPA记录（NULL）的学生。</t>
+  </si>
+  <si>
+    <t>Find students with NULL GPA.</t>
+  </si>
+  <si>
+    <t>查询所有课程中不是必修（is_mandatory=0）且课程学分不是2.0或3.0的。</t>
+  </si>
+  <si>
+    <t>Find courses that are not mandatory and whose credit is not 2.0 or 3.0.</t>
+  </si>
+  <si>
+    <t>查找学生中入学日期早于2020年，且GPA不在3.5到4.0之间的记录。</t>
+  </si>
+  <si>
+    <t>Find students enrolled before 2020 whose GPA is not between 3.5 and 4.0.</t>
+  </si>
+  <si>
+    <t>查询名字包含“小”但不包含“明”的学生。</t>
+  </si>
+  <si>
+    <t>Find students whose names contain ‘小’ but not ‘明’.</t>
+  </si>
+  <si>
+    <t>查询成绩为NULL或成绩大于85的选课记录。</t>
+  </si>
+  <si>
+    <t>Find enrollment records where score is NULL or greater than 85.</t>
+  </si>
+  <si>
+    <t>11–20. 数值函数（ROUND, ABS, CEIL, FLOOR, POWER, SQRT）</t>
+  </si>
+  <si>
+    <t>查询每位教师的工资四舍五入后的值。</t>
+  </si>
+  <si>
+    <t>Show the rounded salary of each teacher.</t>
+  </si>
+  <si>
+    <t>显示所有课程的学分平方值。</t>
+  </si>
+  <si>
+    <t>Display square of credit for each course.</t>
+  </si>
+  <si>
+    <t>显示所有课程学分的平方根，保留两位小数。</t>
+  </si>
+  <si>
+    <t>Show the square root of each course’s credit (rounded to 2 decimals).</t>
+  </si>
+  <si>
+    <t>计算所有学生GPA的绝对值。</t>
+  </si>
+  <si>
+    <t>Calculate the absolute value of each student’s GPA.</t>
+  </si>
+  <si>
+    <t>取所有教师工资的上整和下整值。</t>
+  </si>
+  <si>
+    <t>Get the CEIL and FLOOR values of each teacher’s salary.</t>
+  </si>
+  <si>
+    <t>查询选课成绩与平均成绩的差值的绝对值。</t>
+  </si>
+  <si>
+    <t>Show ABS(score - average score) for each enrollment.</t>
+  </si>
+  <si>
+    <t>显示每门课程学分的立方值。</t>
+  </si>
+  <si>
+    <t>Show the cube (POWER(credit, 3)) of each course’s credit.</t>
+  </si>
+  <si>
+    <t>查询分数四舍五入后大于90的选课记录。</t>
+  </si>
+  <si>
+    <t>Find enrollments where rounded score &gt; 90.</t>
+  </si>
+  <si>
+    <t>显示所有学生GPA的平方根，忽略GPA为NULL的。</t>
+  </si>
+  <si>
+    <t>Show SQRT(GPA) for students with non-NULL GPA.</t>
+  </si>
+  <si>
+    <t>找出分数小于平均值平方根的选课记录。</t>
+  </si>
+  <si>
+    <t>Find enrollments where score &lt; SQRT(AVG(score)).</t>
+  </si>
+  <si>
+    <t>21–30. 字符串处理函数（LENGTH, UPPER, LOWER, SUBSTR, TRIM, REPLACE, INSTR）</t>
+  </si>
+  <si>
+    <t>显示所有学生名字的大写和小写形式。</t>
+  </si>
+  <si>
+    <t>Show UPPER and LOWER names of all students.</t>
+  </si>
+  <si>
+    <t>查询所有课程名长度大于6的课程。</t>
+  </si>
+  <si>
+    <t>Find courses where LENGTH(course_name) &gt; 6.</t>
+  </si>
+  <si>
+    <t>查询包含“编程”关键字的课程名。</t>
+  </si>
+  <si>
+    <t>Find courses where INSTR(course_name, ‘编程’) &gt; 0.</t>
+  </si>
+  <si>
+    <t>显示学生名字的前三个字符。</t>
+  </si>
+  <si>
+    <t>Show the first 3 characters of each student’s name.</t>
+  </si>
+  <si>
+    <t>去除教师名字两端空格后再显示。</t>
+  </si>
+  <si>
+    <t>Show TRIM(name) for all teachers.</t>
+  </si>
+  <si>
+    <t>将课程名中的“编程”替换为“程序设计”。</t>
+  </si>
+  <si>
+    <t>Replace ‘编程’ with ‘程序设计’ in course names.</t>
+  </si>
+  <si>
+    <t>查询名字中包含“红”的学生，其名字长度不小于3。</t>
+  </si>
+  <si>
+    <t>Find students whose name contains ‘红’ and LENGTH(name) ≥ 3.</t>
+  </si>
+  <si>
+    <t>查询长度不等于2的教师职称。</t>
+  </si>
+  <si>
+    <t>Find distinct titles where LENGTH(title) ≠ 2.</t>
+  </si>
+  <si>
+    <t>查询所有课程名中，包含“与”字的位置。</t>
+  </si>
+  <si>
+    <t>Show position of ‘与’ in each course name using INSTR.</t>
+  </si>
+  <si>
+    <t>显示学生名字最后两个字符。</t>
+  </si>
+  <si>
+    <t>Show SUBSTR(name, -2, 2) for each student.</t>
+  </si>
+  <si>
+    <t>31–40. 日期与时间函数（DATE, DATETIME, STRFTIME）</t>
+  </si>
+  <si>
+    <t>查询当前日期是星期几（数字形式0=周日）。</t>
+  </si>
+  <si>
+    <t>What day of the week is today? Use STRFTIME(’%w’, ‘now’).</t>
+  </si>
+  <si>
+    <t>查询今天是一年中的第几天？</t>
+  </si>
+  <si>
+    <t>What day of the year is today? Use STRFTIME(’%j’, ‘now’).</t>
+  </si>
+  <si>
+    <t>显示每位教师入职的年份和月份。</t>
+  </si>
+  <si>
+    <t>Show hire year and month for each teacher.</t>
+  </si>
+  <si>
+    <t>查询入职年份为2018或之后的教师。</t>
+  </si>
+  <si>
+    <t>Find teachers hired in or after 2018.</t>
+  </si>
+  <si>
+    <t>查询所有学生出生月份是2月或3月的。</t>
+  </si>
+  <si>
+    <t>Find students whose birth month is February or March.</t>
+  </si>
+  <si>
+    <t>显示每位学生的出生日期到现在的天数。</t>
+  </si>
+  <si>
+    <t>Show the number of days since each student’s birth date.</t>
+  </si>
+  <si>
+    <t>查询2025年1月1日向前推一个月是哪天？</t>
+  </si>
+  <si>
+    <t>What date is one month before Jan 1, 2025?</t>
+  </si>
+  <si>
+    <t>查询三天前的日期。</t>
+  </si>
+  <si>
+    <t>What was the date 3 days ago?</t>
+  </si>
+  <si>
+    <t>查询当前时间加3小时减15分钟。</t>
+  </si>
+  <si>
+    <t>Show DATETIME(‘now’, ‘+3 hours’, ‘-15 minutes’).</t>
+  </si>
+  <si>
+    <t>查询2025年1月1日加1年减1月的日期。</t>
+  </si>
+  <si>
+    <t>What date is DATE(‘2025-01-01’, ‘+1 year’, ‘-1 month’)?</t>
+  </si>
+  <si>
+    <t>41–50. 综合题（多函数+条件）</t>
+  </si>
+  <si>
+    <t>查询课程名长度大于8且学分的平方大于10的课程。</t>
+  </si>
+  <si>
+    <t>Find courses where LENGTH(course_name) &gt; 8 and POWER(credit, 2) &gt; 10.</t>
+  </si>
+  <si>
+    <t>查询学生中名字长度等于2，GPA四舍五入后为4的记录。</t>
+  </si>
+  <si>
+    <t>Find students whose name length = 2 and rounded GPA = 4.</t>
+  </si>
+  <si>
+    <t>查询教师中，名字中包含“陈”或“赵”，且工资上整后大于9000的。</t>
+  </si>
+  <si>
+    <t>Find teachers whose name includes ‘陈’ or ‘赵’ and CEIL(salary) &gt; 9000.</t>
+  </si>
+  <si>
+    <t>查询学生入学日期早于2021年，且其出生年为偶数。</t>
+  </si>
+  <si>
+    <t>Find students enrolled before 2021 whose birth year is even.</t>
+  </si>
+  <si>
+    <t>查询学生名字包含“刚”或“洁”，且年龄不在20到22之间的记录。</t>
+  </si>
+  <si>
+    <t>Find students whose names include ‘刚’ or ‘洁’ and age NOT BETWEEN 20 AND 22.</t>
+  </si>
+  <si>
+    <t>查询选课成绩大于平均成绩，且其课程为必修课的学生ID。</t>
+  </si>
+  <si>
+    <t>Find student IDs with score &gt; average and enrolled in mandatory courses.</t>
+  </si>
+  <si>
+    <t>查询教师名字中不含“李”，且工资不为NULL的记录。</t>
+  </si>
+  <si>
+    <t>Find teachers whose name does not include ‘李’ and salary IS NOT NULL.</t>
+  </si>
+  <si>
+    <t>查询课程中名字包含“与”且课程时间早于12:00的。</t>
+  </si>
+  <si>
+    <t>Find courses that include ‘与’ in the name and are scheduled before 12:00.</t>
+  </si>
+  <si>
+    <t>查询所有学生的年龄与GPA乘积，结果保留两位小数。</t>
+  </si>
+  <si>
+    <t>Show ROUND(age * GPA, 2) for all students.</t>
+  </si>
+  <si>
+    <t>查询所有学生入学到今天的年数，保留两位小数。</t>
+  </si>
+  <si>
+    <t>Show how many years since each student enrolled (rounded to 2 decimals).</t>
   </si>
 </sst>
 </file>
@@ -3430,6 +3746,10 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3454,11 +3774,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4576,7 +4892,7 @@
   </sheetPr>
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="86" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A56" zoomScale="86" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
@@ -4783,7 +5099,7 @@
       <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="71" t="s">
+      <c r="D28" s="75" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4797,7 +5113,7 @@
       <c r="C29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="71"/>
+      <c r="D29" s="75"/>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="10" t="s">
@@ -4809,7 +5125,7 @@
       <c r="C30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="71"/>
+      <c r="D30" s="75"/>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="10" t="s">
@@ -4821,7 +5137,7 @@
       <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="71"/>
+      <c r="D31" s="75"/>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="10" t="s">
@@ -4833,7 +5149,7 @@
       <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="71"/>
+      <c r="D32" s="75"/>
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="10" t="s">
@@ -4845,7 +5161,7 @@
       <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="71"/>
+      <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" s="10" t="s">
@@ -4857,7 +5173,7 @@
       <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="71"/>
+      <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="10" t="s">
@@ -4869,7 +5185,7 @@
       <c r="C35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="71"/>
+      <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="30">
       <c r="A36" s="10" t="s">
@@ -4881,7 +5197,7 @@
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="71"/>
+      <c r="D36" s="75"/>
     </row>
     <row r="37" spans="1:4" ht="30">
       <c r="A37" s="10" t="s">
@@ -4893,7 +5209,7 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="71"/>
+      <c r="D37" s="75"/>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" s="10" t="s">
@@ -4905,7 +5221,7 @@
       <c r="C38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="71"/>
+      <c r="D38" s="75"/>
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="10" t="s">
@@ -4917,7 +5233,7 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="71"/>
+      <c r="D39" s="75"/>
     </row>
     <row r="40" spans="1:4" ht="30">
       <c r="A40" s="10" t="s">
@@ -4929,7 +5245,7 @@
       <c r="C40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="71"/>
+      <c r="D40" s="75"/>
     </row>
     <row r="41" spans="1:4" ht="30">
       <c r="A41" s="10" t="s">
@@ -4941,7 +5257,7 @@
       <c r="C41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="71"/>
+      <c r="D41" s="75"/>
     </row>
     <row r="42" spans="1:4" ht="30">
       <c r="A42" s="10" t="s">
@@ -4953,7 +5269,7 @@
       <c r="C42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="71"/>
+      <c r="D42" s="75"/>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="10" t="s">
@@ -4965,7 +5281,7 @@
       <c r="C43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="71"/>
+      <c r="D43" s="75"/>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="10" t="s">
@@ -4977,7 +5293,7 @@
       <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="71"/>
+      <c r="D44" s="75"/>
     </row>
     <row r="52" spans="1:5" ht="27">
       <c r="A52" s="3" t="s">
@@ -5045,12 +5361,12 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="23">
-      <c r="A62" s="79" t="s">
+      <c r="A62" s="71" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="23">
-      <c r="A63" s="79" t="s">
+      <c r="A63" s="71" t="s">
         <v>869</v>
       </c>
       <c r="B63" s="42"/>
@@ -5347,10 +5663,10 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="C46" s="72" t="s">
+      <c r="C46" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="D46" s="72"/>
+      <c r="D46" s="76"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="22" t="s">
@@ -5436,7 +5752,9 @@
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>
@@ -5568,7 +5886,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="80" t="s">
         <v>200</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -5582,7 +5900,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="77"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="58" t="s">
         <v>483</v>
       </c>
@@ -5594,7 +5912,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="80" t="s">
         <v>205</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -5608,7 +5926,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="77"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="26" t="s">
         <v>209</v>
       </c>
@@ -5620,7 +5938,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="80" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -5634,7 +5952,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="77"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="26" t="s">
         <v>216</v>
       </c>
@@ -5674,7 +5992,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="80" t="s">
         <v>227</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -5688,7 +6006,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="78"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="26" t="s">
         <v>229</v>
       </c>
@@ -5700,7 +6018,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="77"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="26" t="s">
         <v>232</v>
       </c>
@@ -5740,7 +6058,7 @@
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="77" t="s">
         <v>240</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -5754,7 +6072,7 @@
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="74"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="26" t="s">
         <v>243</v>
       </c>
@@ -5766,7 +6084,7 @@
       </c>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="74"/>
+      <c r="B37" s="78"/>
       <c r="C37" s="26" t="s">
         <v>602</v>
       </c>
@@ -5778,7 +6096,7 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="74"/>
+      <c r="B38" s="78"/>
       <c r="C38" s="26" t="s">
         <v>248</v>
       </c>
@@ -5790,7 +6108,7 @@
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="74"/>
+      <c r="B39" s="78"/>
       <c r="C39" s="26" t="s">
         <v>250</v>
       </c>
@@ -5802,7 +6120,7 @@
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="75"/>
+      <c r="B40" s="79"/>
       <c r="C40" s="26" t="s">
         <v>252</v>
       </c>
@@ -5814,7 +6132,7 @@
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="77" t="s">
         <v>255</v>
       </c>
       <c r="C41" s="26" t="s">
@@ -5828,7 +6146,7 @@
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="74"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="26" t="s">
         <v>259</v>
       </c>
@@ -5840,7 +6158,7 @@
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="74"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="59" t="s">
         <v>604</v>
       </c>
@@ -5855,7 +6173,7 @@
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="74"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="26" t="s">
         <v>603</v>
       </c>
@@ -5867,7 +6185,7 @@
       </c>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="74"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="26" t="s">
         <v>264</v>
       </c>
@@ -5882,7 +6200,7 @@
       </c>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="75"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="26" t="s">
         <v>266</v>
       </c>
@@ -5895,10 +6213,10 @@
       <c r="L46" s="46"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="77" t="s">
         <v>268</v>
       </c>
-      <c r="C47" s="81" t="s">
+      <c r="C47" s="26" t="s">
         <v>269</v>
       </c>
       <c r="D47" s="26" t="s">
@@ -5912,8 +6230,8 @@
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="74"/>
-      <c r="C48" s="81" t="s">
+      <c r="B48" s="78"/>
+      <c r="C48" s="26" t="s">
         <v>272</v>
       </c>
       <c r="D48" s="26" t="s">
@@ -5925,8 +6243,8 @@
       <c r="L48" s="46"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="74"/>
-      <c r="C49" s="81" t="s">
+      <c r="B49" s="78"/>
+      <c r="C49" s="26" t="s">
         <v>275</v>
       </c>
       <c r="D49" s="26" t="s">
@@ -5940,8 +6258,8 @@
       </c>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="74"/>
-      <c r="C50" s="81" t="s">
+      <c r="B50" s="78"/>
+      <c r="C50" s="26" t="s">
         <v>278</v>
       </c>
       <c r="D50" s="26" t="s">
@@ -5953,8 +6271,8 @@
       <c r="L50" s="46"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="74"/>
-      <c r="C51" s="81" t="s">
+      <c r="B51" s="78"/>
+      <c r="C51" s="26" t="s">
         <v>281</v>
       </c>
       <c r="D51" s="26" t="s">
@@ -5968,8 +6286,8 @@
       </c>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="75"/>
-      <c r="C52" s="81" t="s">
+      <c r="B52" s="79"/>
+      <c r="C52" s="26" t="s">
         <v>284</v>
       </c>
       <c r="D52" s="26" t="s">
@@ -5980,10 +6298,10 @@
       </c>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="73" t="s">
+      <c r="B53" s="77" t="s">
         <v>287</v>
       </c>
-      <c r="C53" s="80" t="s">
+      <c r="C53" s="72" t="s">
         <v>872</v>
       </c>
       <c r="D53" s="26" t="s">
@@ -5994,8 +6312,8 @@
       </c>
     </row>
     <row r="54" spans="2:12">
-      <c r="B54" s="74"/>
-      <c r="C54" s="80" t="s">
+      <c r="B54" s="78"/>
+      <c r="C54" s="72" t="s">
         <v>290</v>
       </c>
       <c r="D54" s="26" t="s">
@@ -6006,8 +6324,8 @@
       </c>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="74"/>
-      <c r="C55" s="80" t="s">
+      <c r="B55" s="78"/>
+      <c r="C55" s="72" t="s">
         <v>293</v>
       </c>
       <c r="D55" s="26" t="s">
@@ -6018,8 +6336,8 @@
       </c>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="74"/>
-      <c r="C56" s="80" t="s">
+      <c r="B56" s="78"/>
+      <c r="C56" s="72" t="s">
         <v>296</v>
       </c>
       <c r="D56" s="26" t="s">
@@ -6030,8 +6348,8 @@
       </c>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="75"/>
-      <c r="C57" s="80" t="s">
+      <c r="B57" s="79"/>
+      <c r="C57" s="72" t="s">
         <v>873</v>
       </c>
       <c r="D57" s="26" t="s">
@@ -6042,7 +6360,7 @@
       </c>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="77" t="s">
         <v>301</v>
       </c>
       <c r="C58" s="26" t="s">
@@ -6056,7 +6374,7 @@
       </c>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="74"/>
+      <c r="B59" s="78"/>
       <c r="C59" s="26" t="s">
         <v>305</v>
       </c>
@@ -6068,7 +6386,7 @@
       </c>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="74"/>
+      <c r="B60" s="78"/>
       <c r="C60" s="26" t="s">
         <v>308</v>
       </c>
@@ -6080,7 +6398,7 @@
       </c>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="75"/>
+      <c r="B61" s="79"/>
       <c r="C61" s="26" t="s">
         <v>311</v>
       </c>
@@ -6809,7 +7127,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BA09B4-4C11-4647-8D7F-110373603660}">
-  <dimension ref="A1:AH176"/>
+  <dimension ref="A1:AQ217"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6819,7 +7137,7 @@
     <col min="7" max="7" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="17">
+    <row r="1" spans="1:43" ht="19">
       <c r="A1" t="s">
         <v>403</v>
       </c>
@@ -6838,8 +7156,11 @@
       <c r="AH1" s="1" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" ht="17">
+      <c r="AQ1" s="83" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="17">
       <c r="A2" t="s">
         <v>404</v>
       </c>
@@ -6853,7 +7174,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18">
+    <row r="3" spans="1:43" ht="18">
       <c r="A3" t="s">
         <v>405</v>
       </c>
@@ -6869,8 +7190,11 @@
       <c r="AH3" s="15" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" ht="17">
+      <c r="AQ3" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" ht="17">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -6888,7 +7212,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="18">
+    <row r="5" spans="1:43" ht="18">
       <c r="A5" t="s">
         <v>406</v>
       </c>
@@ -6907,14 +7231,17 @@
       <c r="AH5" s="15" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" ht="17">
+      <c r="AQ5" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" ht="17">
       <c r="B6" s="15"/>
       <c r="H6" s="15" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18">
+    <row r="7" spans="1:43" ht="18">
       <c r="B7" s="15"/>
       <c r="G7" s="42" t="s">
         <v>496</v>
@@ -6931,8 +7258,11 @@
       <c r="AH7" s="1" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" ht="17">
+      <c r="AQ7" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" ht="17">
       <c r="A8" t="s">
         <v>407</v>
       </c>
@@ -6946,7 +7276,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18">
+    <row r="9" spans="1:43" ht="18">
       <c r="A9" t="s">
         <v>408</v>
       </c>
@@ -6957,8 +7287,11 @@
       <c r="AH9" s="15" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" ht="17">
+      <c r="AQ9" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" ht="17">
       <c r="A10" t="s">
         <v>409</v>
       </c>
@@ -6975,7 +7308,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="18">
+    <row r="11" spans="1:43" ht="18">
       <c r="A11" t="s">
         <v>410</v>
       </c>
@@ -6995,8 +7328,11 @@
       <c r="AH11" s="15" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" ht="17">
+      <c r="AQ11" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" ht="17">
       <c r="A12" t="s">
         <v>411</v>
       </c>
@@ -7008,7 +7344,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="18">
+    <row r="13" spans="1:43" ht="18">
       <c r="A13" t="s">
         <v>412</v>
       </c>
@@ -7027,8 +7363,11 @@
       <c r="AH13" s="1" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="14" spans="1:34">
+      <c r="AQ13" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="B14" s="1"/>
       <c r="G14" s="42" t="s">
         <v>502</v>
@@ -7040,7 +7379,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="18">
+    <row r="15" spans="1:43" ht="18">
       <c r="H15" s="15" t="s">
         <v>503</v>
       </c>
@@ -7053,8 +7392,11 @@
       <c r="AH15" s="15" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" ht="17">
+      <c r="AQ15" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" ht="17">
       <c r="A16" t="s">
         <v>413</v>
       </c>
@@ -7071,7 +7413,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="18">
+    <row r="17" spans="1:43" ht="18">
       <c r="A17" t="s">
         <v>410</v>
       </c>
@@ -7090,13 +7432,16 @@
       <c r="AH17" s="15" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="18" spans="1:34">
+      <c r="AQ17" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43">
       <c r="A18" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="17">
+    <row r="19" spans="1:43" ht="17">
       <c r="A19" t="s">
         <v>412</v>
       </c>
@@ -7115,8 +7460,11 @@
       <c r="AH19" s="1" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="20" spans="1:34" ht="17">
+      <c r="AQ19" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" ht="17">
       <c r="B20" s="1"/>
       <c r="H20" s="15" t="s">
         <v>507</v>
@@ -7128,7 +7476,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="20">
+    <row r="21" spans="1:43" ht="20">
       <c r="G21" s="42" t="s">
         <v>508</v>
       </c>
@@ -7141,8 +7489,11 @@
       <c r="AH21" s="15" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="22" spans="1:34" ht="17">
+      <c r="AQ21" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" ht="17">
       <c r="A22" t="s">
         <v>414</v>
       </c>
@@ -7160,7 +7511,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="17">
+    <row r="23" spans="1:43" ht="17">
       <c r="A23" t="s">
         <v>415</v>
       </c>
@@ -7177,8 +7528,11 @@
       <c r="AH23" s="15" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="24" spans="1:34" ht="17">
+      <c r="AQ23" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" ht="17">
       <c r="H24" s="15" t="s">
         <v>511</v>
       </c>
@@ -7186,7 +7540,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:43">
       <c r="A25" t="s">
         <v>416</v>
       </c>
@@ -7203,8 +7557,11 @@
       <c r="AH25" s="1" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="26" spans="1:34" ht="17">
+      <c r="AQ25" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" ht="17">
       <c r="A26" t="s">
         <v>410</v>
       </c>
@@ -7218,7 +7575,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="17">
+    <row r="27" spans="1:43" ht="17">
       <c r="A27" t="s">
         <v>411</v>
       </c>
@@ -7229,8 +7586,11 @@
       <c r="AH27" s="15" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="28" spans="1:34" ht="17">
+      <c r="AQ27" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" ht="17">
       <c r="A28" t="s">
         <v>412</v>
       </c>
@@ -7248,7 +7608,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="17">
+    <row r="29" spans="1:43" ht="17">
       <c r="H29" s="15" t="s">
         <v>514</v>
       </c>
@@ -7258,8 +7618,11 @@
       <c r="AH29" s="15" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="30" spans="1:34" ht="17">
+      <c r="AQ29" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" ht="17">
       <c r="A30" t="s">
         <v>417</v>
       </c>
@@ -7274,7 +7637,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:43">
       <c r="A31" t="s">
         <v>410</v>
       </c>
@@ -7290,8 +7653,11 @@
       <c r="AH31" s="1" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="32" spans="1:34" ht="17">
+      <c r="AQ31" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43" ht="17">
       <c r="A32" t="s">
         <v>411</v>
       </c>
@@ -7306,7 +7672,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="17">
+    <row r="33" spans="1:43" ht="17">
       <c r="A33" t="s">
         <v>412</v>
       </c>
@@ -7320,8 +7686,11 @@
       <c r="AH33" s="15" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="34" spans="1:34" ht="17">
+      <c r="AQ33" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" ht="17">
       <c r="G34" s="42" t="s">
         <v>522</v>
       </c>
@@ -7335,7 +7704,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="17">
+    <row r="35" spans="1:43" ht="17">
       <c r="A35" t="s">
         <v>418</v>
       </c>
@@ -7349,8 +7718,11 @@
       <c r="AH35" s="15" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="36" spans="1:34" ht="17">
+      <c r="AQ35" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43" ht="17">
       <c r="A36" t="s">
         <v>410</v>
       </c>
@@ -7364,7 +7736,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="37" spans="1:34">
+    <row r="37" spans="1:43">
       <c r="A37" t="s">
         <v>411</v>
       </c>
@@ -7377,8 +7749,11 @@
       <c r="AH37" s="1" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="38" spans="1:34">
+      <c r="AQ37" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43">
       <c r="A38" t="s">
         <v>412</v>
       </c>
@@ -7389,7 +7764,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="17">
+    <row r="39" spans="1:43" ht="17">
       <c r="H39" t="s">
         <v>523</v>
       </c>
@@ -7402,8 +7777,11 @@
       <c r="AH39" s="15" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="40" spans="1:34" ht="17">
+      <c r="AQ39" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" ht="17">
       <c r="H40" t="s">
         <v>524</v>
       </c>
@@ -7417,7 +7795,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="41" spans="1:34">
+    <row r="41" spans="1:43">
       <c r="A41" t="s">
         <v>419</v>
       </c>
@@ -7427,8 +7805,11 @@
       <c r="AC41" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="42" spans="1:34">
+      <c r="AQ41" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43">
       <c r="A42" t="s">
         <v>420</v>
       </c>
@@ -7445,7 +7826,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="43" spans="1:34">
+    <row r="43" spans="1:43">
       <c r="A43" t="s">
         <v>421</v>
       </c>
@@ -7459,7 +7840,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="17">
+    <row r="44" spans="1:43" ht="17">
       <c r="A44" t="s">
         <v>410</v>
       </c>
@@ -7473,7 +7854,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="17">
+    <row r="45" spans="1:43" ht="19">
       <c r="A45" t="s">
         <v>411</v>
       </c>
@@ -7490,8 +7871,11 @@
       <c r="AH45" s="15" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="46" spans="1:34" ht="17">
+      <c r="AQ45" s="83" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43" ht="17">
       <c r="A46" t="s">
         <v>412</v>
       </c>
@@ -7505,7 +7889,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="17">
+    <row r="47" spans="1:43" ht="17">
       <c r="B47" s="15"/>
       <c r="H47" t="s">
         <v>531</v>
@@ -7516,8 +7900,11 @@
       <c r="AC47" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="48" spans="1:34" ht="17">
+      <c r="AQ47" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43" ht="17">
       <c r="B48" s="15"/>
       <c r="W48" t="s">
         <v>596</v>
@@ -7529,7 +7916,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="49" spans="1:34">
+    <row r="49" spans="1:43">
       <c r="A49" t="s">
         <v>422</v>
       </c>
@@ -7542,8 +7929,11 @@
       <c r="AC49" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="50" spans="1:34" ht="17">
+      <c r="AQ49" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43" ht="17">
       <c r="A50" t="s">
         <v>410</v>
       </c>
@@ -7558,7 +7948,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="17">
+    <row r="51" spans="1:43" ht="17">
       <c r="A51" t="s">
         <v>411</v>
       </c>
@@ -7571,8 +7961,11 @@
       <c r="AH51" s="15" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="52" spans="1:34" ht="17">
+      <c r="AQ51" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43" ht="17">
       <c r="A52" t="s">
         <v>412</v>
       </c>
@@ -7587,7 +7980,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="53" spans="1:34" ht="17">
+    <row r="53" spans="1:43" ht="17">
       <c r="B53" s="15"/>
       <c r="H53" t="s">
         <v>535</v>
@@ -7601,8 +7994,11 @@
       <c r="AH53" s="1" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="54" spans="1:34">
+      <c r="AQ53" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43">
       <c r="A54" t="s">
         <v>423</v>
       </c>
@@ -7613,7 +8009,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="55" spans="1:34" ht="17">
+    <row r="55" spans="1:43" ht="17">
       <c r="A55" t="s">
         <v>424</v>
       </c>
@@ -7627,8 +8023,11 @@
       <c r="AH55" s="15" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="56" spans="1:34" ht="17">
+      <c r="AQ55" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="56" spans="1:43" ht="17">
       <c r="A56" t="s">
         <v>425</v>
       </c>
@@ -7642,7 +8041,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="57" spans="1:34" ht="17">
+    <row r="57" spans="1:43" ht="17">
       <c r="A57" t="s">
         <v>426</v>
       </c>
@@ -7659,8 +8058,11 @@
       <c r="AH57" s="15" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="58" spans="1:34" ht="17">
+      <c r="AQ57" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="58" spans="1:43" ht="17">
       <c r="A58" t="s">
         <v>410</v>
       </c>
@@ -7675,7 +8077,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="59" spans="1:34">
+    <row r="59" spans="1:43">
       <c r="A59" t="s">
         <v>411</v>
       </c>
@@ -7691,8 +8093,11 @@
       <c r="AH59" s="1" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="60" spans="1:34">
+      <c r="AQ59" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="60" spans="1:43">
       <c r="A60" t="s">
         <v>412</v>
       </c>
@@ -7704,15 +8109,18 @@
         <v>576</v>
       </c>
     </row>
-    <row r="61" spans="1:34" ht="17">
+    <row r="61" spans="1:43" ht="17">
       <c r="AC61" t="s">
         <v>598</v>
       </c>
       <c r="AH61" s="15" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="62" spans="1:34" ht="17">
+      <c r="AQ61" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="62" spans="1:43" ht="17">
       <c r="A62" t="s">
         <v>427</v>
       </c>
@@ -7726,7 +8134,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="63" spans="1:34" ht="17">
+    <row r="63" spans="1:43" ht="17">
       <c r="A63" t="s">
         <v>410</v>
       </c>
@@ -7739,8 +8147,11 @@
       <c r="AH63" s="15" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="64" spans="1:34">
+      <c r="AQ63" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="64" spans="1:43">
       <c r="A64" t="s">
         <v>411</v>
       </c>
@@ -7751,7 +8162,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="65" spans="1:34">
+    <row r="65" spans="1:43">
       <c r="A65" t="s">
         <v>412</v>
       </c>
@@ -7761,8 +8172,11 @@
       <c r="AH65" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="66" spans="1:34">
+      <c r="AQ65" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="66" spans="1:43">
       <c r="H66" t="s">
         <v>542</v>
       </c>
@@ -7770,7 +8184,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="17">
+    <row r="67" spans="1:43" ht="17">
       <c r="A67" t="s">
         <v>428</v>
       </c>
@@ -7783,8 +8197,11 @@
       <c r="AH67" s="15" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="68" spans="1:34" ht="17">
+      <c r="AQ67" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="68" spans="1:43" ht="17">
       <c r="A68" t="s">
         <v>429</v>
       </c>
@@ -7795,7 +8212,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="17">
+    <row r="69" spans="1:43" ht="17">
       <c r="A69" t="s">
         <v>430</v>
       </c>
@@ -7808,8 +8225,11 @@
       <c r="AH69" s="15" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="70" spans="1:34">
+      <c r="AQ69" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="70" spans="1:43">
       <c r="A70" t="s">
         <v>431</v>
       </c>
@@ -7817,7 +8237,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="71" spans="1:34">
+    <row r="71" spans="1:43">
       <c r="A71" t="s">
         <v>410</v>
       </c>
@@ -7827,8 +8247,11 @@
       <c r="AH71" s="1" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="72" spans="1:34">
+      <c r="AQ71" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="72" spans="1:43">
       <c r="A72" t="s">
         <v>411</v>
       </c>
@@ -7839,7 +8262,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="73" spans="1:34" ht="17">
+    <row r="73" spans="1:43" ht="17">
       <c r="A73" t="s">
         <v>412</v>
       </c>
@@ -7850,8 +8273,11 @@
       <c r="AH73" s="15" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="74" spans="1:34" ht="17">
+      <c r="AQ73" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="74" spans="1:43" ht="17">
       <c r="H74" t="s">
         <v>547</v>
       </c>
@@ -7862,7 +8288,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="17">
+    <row r="75" spans="1:43" ht="17">
       <c r="B75" s="15"/>
       <c r="AC75" t="s">
         <v>614</v>
@@ -7870,8 +8296,11 @@
       <c r="AH75" s="15" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="76" spans="1:34" ht="17">
+      <c r="AQ75" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="76" spans="1:43" ht="17">
       <c r="A76" t="s">
         <v>432</v>
       </c>
@@ -7880,7 +8309,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="77" spans="1:34" ht="17">
+    <row r="77" spans="1:43" ht="17">
       <c r="A77" t="s">
         <v>433</v>
       </c>
@@ -7891,14 +8320,17 @@
       <c r="AH77" s="1" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="78" spans="1:34" ht="17">
+      <c r="AQ77" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="78" spans="1:43" ht="17">
       <c r="A78" t="s">
         <v>434</v>
       </c>
       <c r="B78" s="15"/>
     </row>
-    <row r="79" spans="1:34" ht="17">
+    <row r="79" spans="1:43" ht="17">
       <c r="A79" t="s">
         <v>410</v>
       </c>
@@ -7909,8 +8341,11 @@
       <c r="AH79" s="15" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="80" spans="1:34" ht="17">
+      <c r="AQ79" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="80" spans="1:43" ht="17">
       <c r="A80" t="s">
         <v>411</v>
       </c>
@@ -7922,7 +8357,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="81" spans="1:34" ht="17">
+    <row r="81" spans="1:43" ht="17">
       <c r="A81" t="s">
         <v>412</v>
       </c>
@@ -7932,14 +8367,17 @@
       <c r="AH81" s="15" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="82" spans="1:34">
+      <c r="AQ81" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="82" spans="1:43">
       <c r="B82" s="1"/>
       <c r="AC82" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="83" spans="1:34">
+    <row r="83" spans="1:43">
       <c r="A83" t="s">
         <v>435</v>
       </c>
@@ -7949,8 +8387,11 @@
       <c r="AH83" s="1" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="84" spans="1:34">
+      <c r="AQ83" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="84" spans="1:43">
       <c r="A84" t="s">
         <v>410</v>
       </c>
@@ -7958,7 +8399,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="85" spans="1:34" ht="17">
+    <row r="85" spans="1:43" ht="17">
       <c r="A85" t="s">
         <v>411</v>
       </c>
@@ -7968,8 +8409,11 @@
       <c r="AH85" s="15" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="86" spans="1:34" ht="17">
+      <c r="AQ85" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="86" spans="1:43" ht="17">
       <c r="A86" t="s">
         <v>412</v>
       </c>
@@ -7977,7 +8421,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="87" spans="1:34" ht="17">
+    <row r="87" spans="1:43" ht="17">
       <c r="AC87" t="s">
         <v>620</v>
       </c>
@@ -7985,7 +8429,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="88" spans="1:34">
+    <row r="88" spans="1:43">
       <c r="A88" t="s">
         <v>436</v>
       </c>
@@ -7993,7 +8437,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="89" spans="1:34">
+    <row r="89" spans="1:43" ht="19">
       <c r="A89" t="s">
         <v>410</v>
       </c>
@@ -8003,13 +8447,16 @@
       <c r="AH89" s="1" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="90" spans="1:34">
+      <c r="AQ89" s="83" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="90" spans="1:43">
       <c r="A90" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="91" spans="1:34" ht="17">
+    <row r="91" spans="1:43" ht="17">
       <c r="A91" t="s">
         <v>412</v>
       </c>
@@ -8019,8 +8466,11 @@
       <c r="AH91" s="15" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="92" spans="1:34" ht="17">
+      <c r="AQ91" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="92" spans="1:43" ht="17">
       <c r="AC92" t="s">
         <v>623</v>
       </c>
@@ -8028,7 +8478,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="93" spans="1:34" ht="17">
+    <row r="93" spans="1:43" ht="17">
       <c r="A93" t="s">
         <v>437</v>
       </c>
@@ -8038,13 +8488,16 @@
       <c r="AH93" s="15" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="94" spans="1:34">
+      <c r="AQ93" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="94" spans="1:43">
       <c r="A94" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="95" spans="1:34">
+    <row r="95" spans="1:43">
       <c r="A95" t="s">
         <v>439</v>
       </c>
@@ -8054,8 +8507,11 @@
       <c r="AH95" s="1" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="96" spans="1:34">
+      <c r="AQ95" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="96" spans="1:43">
       <c r="A96" t="s">
         <v>410</v>
       </c>
@@ -8063,7 +8519,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="97" spans="1:34" ht="17">
+    <row r="97" spans="1:43" ht="17">
       <c r="A97" t="s">
         <v>411</v>
       </c>
@@ -8073,8 +8529,11 @@
       <c r="AH97" s="15" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="98" spans="1:34" ht="17">
+      <c r="AQ97" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="98" spans="1:43" ht="17">
       <c r="A98" t="s">
         <v>412</v>
       </c>
@@ -8082,7 +8541,12 @@
         <v>447</v>
       </c>
     </row>
-    <row r="100" spans="1:34">
+    <row r="99" spans="1:43">
+      <c r="AQ99" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="100" spans="1:43">
       <c r="A100" t="s">
         <v>440</v>
       </c>
@@ -8090,12 +8554,15 @@
         <v>675</v>
       </c>
     </row>
-    <row r="101" spans="1:34">
+    <row r="101" spans="1:43">
       <c r="A101" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="102" spans="1:34" ht="17">
+      <c r="AQ101" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="102" spans="1:43" ht="17">
       <c r="A102" t="s">
         <v>411</v>
       </c>
@@ -8103,33 +8570,47 @@
         <v>676</v>
       </c>
     </row>
-    <row r="103" spans="1:34" ht="17">
+    <row r="103" spans="1:43" ht="17">
       <c r="A103" t="s">
         <v>412</v>
       </c>
       <c r="AH103" s="15" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="105" spans="1:34">
+      <c r="AQ103" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="105" spans="1:43">
       <c r="AH105" s="1" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="107" spans="1:34" ht="17">
+      <c r="AQ105" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="107" spans="1:43" ht="17">
       <c r="A107" t="s">
         <v>441</v>
       </c>
       <c r="AH107" s="15" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="108" spans="1:34" ht="17">
+      <c r="AQ107" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="108" spans="1:43" ht="17">
       <c r="AH108" s="15" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="110" spans="1:34">
+    <row r="109" spans="1:43">
+      <c r="AQ109" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="110" spans="1:43">
       <c r="A110" t="s">
         <v>442</v>
       </c>
@@ -8137,56 +8618,73 @@
         <v>679</v>
       </c>
     </row>
-    <row r="112" spans="1:34" ht="17">
+    <row r="111" spans="1:43">
+      <c r="AQ111" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="112" spans="1:43" ht="17">
       <c r="AH112" s="15" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="113" spans="1:34" ht="17">
+    <row r="113" spans="1:43" ht="17">
       <c r="A113" t="s">
         <v>443</v>
       </c>
       <c r="AH113" s="15" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="114" spans="1:34">
+      <c r="AQ113" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="114" spans="1:43">
       <c r="A114" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="115" spans="1:34">
+    <row r="115" spans="1:43">
       <c r="A115" t="s">
         <v>445</v>
       </c>
       <c r="AH115" s="1" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="116" spans="1:34">
+      <c r="AQ115" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="116" spans="1:43">
       <c r="A116" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="117" spans="1:34" ht="17">
+    <row r="117" spans="1:43" ht="17">
       <c r="A117" t="s">
         <v>447</v>
       </c>
       <c r="AH117" s="15" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="118" spans="1:34" ht="17">
+      <c r="AQ117" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="118" spans="1:43" ht="17">
       <c r="AH118" s="15" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="119" spans="1:34">
+    <row r="119" spans="1:43">
       <c r="A119" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="120" spans="1:34">
+      <c r="AQ119" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="120" spans="1:43">
       <c r="A120" t="s">
         <v>449</v>
       </c>
@@ -8194,7 +8692,12 @@
         <v>683</v>
       </c>
     </row>
-    <row r="122" spans="1:34" ht="17">
+    <row r="121" spans="1:43">
+      <c r="AQ121" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="122" spans="1:43" ht="17">
       <c r="A122" t="s">
         <v>450</v>
       </c>
@@ -8202,33 +8705,42 @@
         <v>684</v>
       </c>
     </row>
-    <row r="123" spans="1:34" ht="17">
+    <row r="123" spans="1:43" ht="17">
       <c r="A123" t="s">
         <v>451</v>
       </c>
       <c r="AH123" s="15" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="125" spans="1:34">
+      <c r="AQ123" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="125" spans="1:43">
       <c r="A125" t="s">
         <v>452</v>
       </c>
       <c r="AH125" s="1" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="126" spans="1:34">
+      <c r="AQ125" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="126" spans="1:43">
       <c r="A126" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="127" spans="1:34" ht="17">
+    <row r="127" spans="1:43" ht="17">
       <c r="AH127" s="15" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="128" spans="1:34" ht="17">
+      <c r="AQ127" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="128" spans="1:43" ht="17">
       <c r="A128" t="s">
         <v>453</v>
       </c>
@@ -8236,12 +8748,15 @@
         <v>447</v>
       </c>
     </row>
-    <row r="129" spans="1:34">
+    <row r="129" spans="1:43">
       <c r="A129" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="130" spans="1:34">
+      <c r="AQ129" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="130" spans="1:43">
       <c r="A130" t="s">
         <v>455</v>
       </c>
@@ -8249,25 +8764,28 @@
         <v>687</v>
       </c>
     </row>
-    <row r="131" spans="1:34">
+    <row r="131" spans="1:43">
       <c r="A131" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="132" spans="1:34" ht="17">
+    <row r="132" spans="1:43" ht="17">
       <c r="AH132" s="15" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="133" spans="1:34" ht="17">
+    <row r="133" spans="1:43" ht="19">
       <c r="A133" t="s">
         <v>456</v>
       </c>
       <c r="AH133" s="15" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="134" spans="1:34" ht="17">
+      <c r="AQ133" s="83" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="134" spans="1:43" ht="17">
       <c r="A134" t="s">
         <v>457</v>
       </c>
@@ -8275,33 +8793,42 @@
         <v>688</v>
       </c>
     </row>
-    <row r="135" spans="1:34" ht="17">
+    <row r="135" spans="1:43" ht="17">
       <c r="AH135" s="15" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="136" spans="1:34">
+      <c r="AQ135" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="136" spans="1:43">
       <c r="A136" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="137" spans="1:34">
+    <row r="137" spans="1:43">
       <c r="A137" t="s">
         <v>447</v>
       </c>
       <c r="AH137" s="1" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="139" spans="1:34" ht="17">
+      <c r="AQ137" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="139" spans="1:43" ht="17">
       <c r="A139" t="s">
         <v>459</v>
       </c>
       <c r="AH139" s="15" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="140" spans="1:34" ht="17">
+      <c r="AQ139" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="140" spans="1:43" ht="17">
       <c r="A140" t="s">
         <v>460</v>
       </c>
@@ -8309,12 +8836,15 @@
         <v>628</v>
       </c>
     </row>
-    <row r="141" spans="1:34" ht="17">
+    <row r="141" spans="1:43" ht="17">
       <c r="AH141" s="15" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="142" spans="1:34" ht="17">
+      <c r="AQ141" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="142" spans="1:43" ht="17">
       <c r="A142" t="s">
         <v>461</v>
       </c>
@@ -8322,134 +8852,293 @@
         <v>693</v>
       </c>
     </row>
-    <row r="143" spans="1:34">
+    <row r="143" spans="1:43">
       <c r="A143" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="AQ143" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="145" spans="1:43">
       <c r="A145" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="AQ145" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="147" spans="1:43">
       <c r="A147" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="AQ147" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="148" spans="1:43">
       <c r="A148" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="149" spans="1:43">
+      <c r="AQ149" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="150" spans="1:43">
       <c r="A150" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:43">
       <c r="A151" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="AQ151" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="153" spans="1:43">
       <c r="A153" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="AQ153" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="154" spans="1:43">
       <c r="A154" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:43">
       <c r="A155" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="AQ155" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="156" spans="1:43">
       <c r="A156" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="157" spans="1:43">
+      <c r="AQ157" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="158" spans="1:43">
       <c r="A158" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:43">
       <c r="A159" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="AQ159" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="160" spans="1:43">
       <c r="A160" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:43">
       <c r="A161" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="AQ161" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="163" spans="1:43">
       <c r="A163" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="AQ163" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="164" spans="1:43">
       <c r="A164" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:43">
       <c r="A165" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="AQ165" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="166" spans="1:43">
       <c r="A166" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="167" spans="1:43">
+      <c r="AQ167" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="168" spans="1:43">
       <c r="A168" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:43">
       <c r="A169" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="AQ169" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="170" spans="1:43">
       <c r="A170" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:43">
       <c r="A171" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="AQ171" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="173" spans="1:43">
       <c r="A173" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="AQ173" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="174" spans="1:43">
       <c r="A174" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:43">
       <c r="A175" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:43">
       <c r="A176" t="s">
         <v>447</v>
+      </c>
+    </row>
+    <row r="177" spans="43:43" ht="19">
+      <c r="AQ177" s="83" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="179" spans="43:43">
+      <c r="AQ179" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="181" spans="43:43">
+      <c r="AQ181" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="184" spans="43:43">
+      <c r="AQ184" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="186" spans="43:43">
+      <c r="AQ186" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="187" spans="43:43">
+      <c r="AQ187" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="189" spans="43:43">
+      <c r="AQ189" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="191" spans="43:43">
+      <c r="AQ191" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="193" spans="43:43">
+      <c r="AQ193" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="195" spans="43:43">
+      <c r="AQ195" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="197" spans="43:43">
+      <c r="AQ197" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="199" spans="43:43">
+      <c r="AQ199" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="201" spans="43:43">
+      <c r="AQ201" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="203" spans="43:43">
+      <c r="AQ203" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="205" spans="43:43">
+      <c r="AQ205" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="207" spans="43:43">
+      <c r="AQ207" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="209" spans="43:43">
+      <c r="AQ209" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="211" spans="43:43">
+      <c r="AQ211" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="213" spans="43:43">
+      <c r="AQ213" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="215" spans="43:43">
+      <c r="AQ215" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="217" spans="43:43">
+      <c r="AQ217" t="s">
+        <v>979</v>
       </c>
     </row>
   </sheetData>
@@ -8464,8 +9153,8 @@
   </sheetPr>
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31" defaultRowHeight="16"/>
@@ -9056,6 +9745,9 @@
       <c r="E1" s="68" t="s">
         <v>757</v>
       </c>
+      <c r="F1" s="72" t="s">
+        <v>872</v>
+      </c>
       <c r="G1" s="69" t="s">
         <v>810</v>
       </c>
@@ -9076,8 +9768,11 @@
       <c r="E2" s="64">
         <v>1</v>
       </c>
+      <c r="F2" s="72" t="s">
+        <v>290</v>
+      </c>
       <c r="G2" s="70"/>
-      <c r="H2" s="82" t="s">
+      <c r="H2" s="73" t="s">
         <v>874</v>
       </c>
     </row>
@@ -9097,8 +9792,11 @@
       <c r="E3" s="64">
         <v>2</v>
       </c>
+      <c r="F3" s="72" t="s">
+        <v>293</v>
+      </c>
       <c r="G3" s="65"/>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="73" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9114,8 +9812,11 @@
         <v>761</v>
       </c>
       <c r="E4" s="64"/>
+      <c r="F4" s="72" t="s">
+        <v>296</v>
+      </c>
       <c r="G4" s="65"/>
-      <c r="H4" s="82" t="s">
+      <c r="H4" s="73" t="s">
         <v>811</v>
       </c>
     </row>
@@ -9133,8 +9834,11 @@
       <c r="E5" s="64">
         <v>3</v>
       </c>
+      <c r="F5" s="72" t="s">
+        <v>873</v>
+      </c>
       <c r="G5" s="65"/>
-      <c r="H5" s="83"/>
+      <c r="H5" s="74"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="64">
@@ -9153,7 +9857,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="70"/>
-      <c r="H6" s="83"/>
+      <c r="H6" s="74"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="64">
@@ -10430,4 +11134,817 @@
   <autoFilter ref="A1:E51" xr:uid="{EE6A4569-7AEF-904E-A35E-2FEE8FCAFC15}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05B7C55-8519-1744-A6F4-6D9438227DA6}">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24">
+      <c r="A1" s="68" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>754</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>755</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>756</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24">
+      <c r="A2" s="64">
+        <v>3001</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>758</v>
+      </c>
+      <c r="C2" s="64">
+        <v>20</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E2" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24">
+      <c r="A3" s="64">
+        <v>3005</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>763</v>
+      </c>
+      <c r="C3" s="64">
+        <v>19</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E3" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24">
+      <c r="A4" s="64">
+        <v>3010</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>768</v>
+      </c>
+      <c r="C4" s="64">
+        <v>22</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E4" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24">
+      <c r="A5" s="64">
+        <v>3012</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>770</v>
+      </c>
+      <c r="C5" s="64">
+        <v>25</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E5" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24">
+      <c r="A6" s="64">
+        <v>3015</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>773</v>
+      </c>
+      <c r="C6" s="64">
+        <v>21</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E6" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24">
+      <c r="A7" s="64">
+        <v>3017</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>775</v>
+      </c>
+      <c r="C7" s="64">
+        <v>22</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E7" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24">
+      <c r="A8" s="64">
+        <v>3021</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>780</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E8" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24">
+      <c r="A9" s="64">
+        <v>3024</v>
+      </c>
+      <c r="B9" s="64" t="s">
+        <v>783</v>
+      </c>
+      <c r="C9" s="64">
+        <v>22</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E9" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24">
+      <c r="A10" s="64">
+        <v>3027</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>786</v>
+      </c>
+      <c r="C10" s="64">
+        <v>25</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E10" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24">
+      <c r="A11" s="64">
+        <v>3030</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>789</v>
+      </c>
+      <c r="C11" s="64">
+        <v>18</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E11" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24">
+      <c r="A12" s="64">
+        <v>3033</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>792</v>
+      </c>
+      <c r="C12" s="64">
+        <v>28</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E12" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24">
+      <c r="A13" s="64">
+        <v>3038</v>
+      </c>
+      <c r="B13" s="64" t="s">
+        <v>797</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E13" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24">
+      <c r="A14" s="64">
+        <v>3040</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>799</v>
+      </c>
+      <c r="C14" s="64">
+        <v>20</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E14" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24">
+      <c r="A15" s="64">
+        <v>3043</v>
+      </c>
+      <c r="B15" s="64" t="s">
+        <v>802</v>
+      </c>
+      <c r="C15" s="64">
+        <v>26</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E15" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24">
+      <c r="A16" s="64">
+        <v>3045</v>
+      </c>
+      <c r="B16" s="64" t="s">
+        <v>804</v>
+      </c>
+      <c r="C16" s="64">
+        <v>20</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E16" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24">
+      <c r="A17" s="64">
+        <v>3049</v>
+      </c>
+      <c r="B17" s="64" t="s">
+        <v>808</v>
+      </c>
+      <c r="C17" s="64">
+        <v>23</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E17" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24">
+      <c r="A19" s="68" t="s">
+        <v>753</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>754</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>755</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>756</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24">
+      <c r="A20" s="64">
+        <v>3002</v>
+      </c>
+      <c r="B20" s="64" t="s">
+        <v>760</v>
+      </c>
+      <c r="C20" s="64">
+        <v>21</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E20" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24">
+      <c r="A21" s="64">
+        <v>3006</v>
+      </c>
+      <c r="B21" s="64" t="s">
+        <v>764</v>
+      </c>
+      <c r="C21" s="64">
+        <v>24</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E21" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24">
+      <c r="A22" s="64">
+        <v>3009</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>767</v>
+      </c>
+      <c r="C22" s="64">
+        <v>20</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E22" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24">
+      <c r="A23" s="64">
+        <v>3013</v>
+      </c>
+      <c r="B23" s="64" t="s">
+        <v>771</v>
+      </c>
+      <c r="C23" s="64">
+        <v>20</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E23" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24">
+      <c r="A24" s="64">
+        <v>3016</v>
+      </c>
+      <c r="B24" s="64" t="s">
+        <v>774</v>
+      </c>
+      <c r="C24" s="64">
+        <v>30</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E24" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24">
+      <c r="A25" s="64">
+        <v>3018</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>776</v>
+      </c>
+      <c r="C25" s="64">
+        <v>23</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="E25" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24">
+      <c r="A26" s="64">
+        <v>3022</v>
+      </c>
+      <c r="B26" s="64" t="s">
+        <v>781</v>
+      </c>
+      <c r="C26" s="64">
+        <v>20</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E26" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24">
+      <c r="A27" s="64">
+        <v>3025</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>784</v>
+      </c>
+      <c r="C27" s="64">
+        <v>20</v>
+      </c>
+      <c r="D27" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E27" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24">
+      <c r="A28" s="64">
+        <v>3029</v>
+      </c>
+      <c r="B28" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="C28" s="64">
+        <v>24</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E28" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24">
+      <c r="A29" s="64">
+        <v>3032</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>791</v>
+      </c>
+      <c r="C29" s="64">
+        <v>19</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E29" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24">
+      <c r="A30" s="64">
+        <v>3036</v>
+      </c>
+      <c r="B30" s="64" t="s">
+        <v>795</v>
+      </c>
+      <c r="C30" s="64">
+        <v>20</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E30" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="24">
+      <c r="A31" s="64">
+        <v>3039</v>
+      </c>
+      <c r="B31" s="64" t="s">
+        <v>798</v>
+      </c>
+      <c r="C31" s="64">
+        <v>21</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E31" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="24">
+      <c r="A32" s="64">
+        <v>3042</v>
+      </c>
+      <c r="B32" s="64" t="s">
+        <v>801</v>
+      </c>
+      <c r="C32" s="64">
+        <v>24</v>
+      </c>
+      <c r="D32" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E32" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24">
+      <c r="A33" s="64">
+        <v>3046</v>
+      </c>
+      <c r="B33" s="64" t="s">
+        <v>805</v>
+      </c>
+      <c r="C33" s="64">
+        <v>19</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E33" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24">
+      <c r="A34" s="64">
+        <v>3050</v>
+      </c>
+      <c r="B34" s="64" t="s">
+        <v>809</v>
+      </c>
+      <c r="C34" s="64">
+        <v>21</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E34" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="24">
+      <c r="A36" s="68" t="s">
+        <v>753</v>
+      </c>
+      <c r="B36" s="68" t="s">
+        <v>754</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>755</v>
+      </c>
+      <c r="D36" s="68" t="s">
+        <v>756</v>
+      </c>
+      <c r="E36" s="68" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24">
+      <c r="A37" s="64">
+        <v>3004</v>
+      </c>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64">
+        <v>22</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E37" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24">
+      <c r="A38" s="64">
+        <v>3007</v>
+      </c>
+      <c r="B38" s="64" t="s">
+        <v>765</v>
+      </c>
+      <c r="C38" s="64">
+        <v>20</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E38" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="24">
+      <c r="A39" s="64">
+        <v>3011</v>
+      </c>
+      <c r="B39" s="64" t="s">
+        <v>769</v>
+      </c>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E39" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="24">
+      <c r="A40" s="64">
+        <v>3014</v>
+      </c>
+      <c r="B40" s="64" t="s">
+        <v>772</v>
+      </c>
+      <c r="C40" s="64">
+        <v>28</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E40" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24">
+      <c r="A41" s="64">
+        <v>3020</v>
+      </c>
+      <c r="B41" s="64" t="s">
+        <v>779</v>
+      </c>
+      <c r="C41" s="64">
+        <v>19</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E41" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="24">
+      <c r="A42" s="64">
+        <v>3023</v>
+      </c>
+      <c r="B42" s="64" t="s">
+        <v>782</v>
+      </c>
+      <c r="C42" s="64">
+        <v>21</v>
+      </c>
+      <c r="D42" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E42" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="24">
+      <c r="A43" s="64">
+        <v>3026</v>
+      </c>
+      <c r="B43" s="64" t="s">
+        <v>785</v>
+      </c>
+      <c r="C43" s="64">
+        <v>23</v>
+      </c>
+      <c r="D43" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E43" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24">
+      <c r="A44" s="64">
+        <v>3031</v>
+      </c>
+      <c r="B44" s="64" t="s">
+        <v>790</v>
+      </c>
+      <c r="C44" s="64">
+        <v>27</v>
+      </c>
+      <c r="D44" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E44" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="24">
+      <c r="A45" s="64">
+        <v>3034</v>
+      </c>
+      <c r="B45" s="64" t="s">
+        <v>793</v>
+      </c>
+      <c r="C45" s="64">
+        <v>21</v>
+      </c>
+      <c r="D45" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E45" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24">
+      <c r="A46" s="64">
+        <v>3037</v>
+      </c>
+      <c r="B46" s="64" t="s">
+        <v>796</v>
+      </c>
+      <c r="C46" s="64">
+        <v>23</v>
+      </c>
+      <c r="D46" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E46" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="24">
+      <c r="A47" s="64">
+        <v>3041</v>
+      </c>
+      <c r="B47" s="64" t="s">
+        <v>800</v>
+      </c>
+      <c r="C47" s="64">
+        <v>29</v>
+      </c>
+      <c r="D47" s="64" t="s">
+        <v>761</v>
+      </c>
+      <c r="E47" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24">
+      <c r="A48" s="64">
+        <v>3044</v>
+      </c>
+      <c r="B48" s="64" t="s">
+        <v>803</v>
+      </c>
+      <c r="C48" s="64">
+        <v>22</v>
+      </c>
+      <c r="D48" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E48" s="64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="24">
+      <c r="A49" s="64">
+        <v>3048</v>
+      </c>
+      <c r="B49" s="64" t="s">
+        <v>807</v>
+      </c>
+      <c r="C49" s="64">
+        <v>28</v>
+      </c>
+      <c r="D49" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="E49" s="64">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor Credit Card project structure and add sample data
Removed redundant files from Beginner/Project and consolidated schema and data into Project/Credit Card. Added INSERT_DATA script with sample categories, states, cities, merchants, customers, and transactions. Updated Create_Table for improved schema clarity. Added SQL review script for Lec_7. Updated Arena of Valor and Credit Card database files and slides.
</commit_message>
<xml_diff>
--- a/Beginner/Slides/Lec_5_6.xlsx
+++ b/Beginner/Slides/Lec_5_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238C8BC3-B43B-1D42-8827-F342E8751196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1A653A-5707-9E45-80E9-20AA6FC24B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="2" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL" sheetId="6" r:id="rId1"/>
@@ -3751,7 +3751,6 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3785,6 +3784,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4861,8 +4861,8 @@
   </sheetPr>
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A63" sqref="A62:A63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5068,7 +5068,7 @@
       <c r="C28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="78" t="s">
+      <c r="D28" s="77" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       <c r="C29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="78"/>
+      <c r="D29" s="77"/>
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" s="10" t="s">
@@ -5094,7 +5094,7 @@
       <c r="C30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="78"/>
+      <c r="D30" s="77"/>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="10" t="s">
@@ -5106,7 +5106,7 @@
       <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="78"/>
+      <c r="D31" s="77"/>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" s="10" t="s">
@@ -5118,7 +5118,7 @@
       <c r="C32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="78"/>
+      <c r="D32" s="77"/>
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="10" t="s">
@@ -5130,7 +5130,7 @@
       <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="78"/>
+      <c r="D33" s="77"/>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" s="10" t="s">
@@ -5142,7 +5142,7 @@
       <c r="C34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="78"/>
+      <c r="D34" s="77"/>
     </row>
     <row r="35" spans="1:4" ht="30">
       <c r="A35" s="10" t="s">
@@ -5154,7 +5154,7 @@
       <c r="C35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="78"/>
+      <c r="D35" s="77"/>
     </row>
     <row r="36" spans="1:4" ht="30">
       <c r="A36" s="10" t="s">
@@ -5166,7 +5166,7 @@
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="78"/>
+      <c r="D36" s="77"/>
     </row>
     <row r="37" spans="1:4" ht="30">
       <c r="A37" s="10" t="s">
@@ -5178,7 +5178,7 @@
       <c r="C37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="78"/>
+      <c r="D37" s="77"/>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" s="10" t="s">
@@ -5190,7 +5190,7 @@
       <c r="C38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="78"/>
+      <c r="D38" s="77"/>
     </row>
     <row r="39" spans="1:4" ht="30">
       <c r="A39" s="10" t="s">
@@ -5202,7 +5202,7 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="78"/>
+      <c r="D39" s="77"/>
     </row>
     <row r="40" spans="1:4" ht="30">
       <c r="A40" s="10" t="s">
@@ -5214,7 +5214,7 @@
       <c r="C40" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="78"/>
+      <c r="D40" s="77"/>
     </row>
     <row r="41" spans="1:4" ht="30">
       <c r="A41" s="10" t="s">
@@ -5226,7 +5226,7 @@
       <c r="C41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="78"/>
+      <c r="D41" s="77"/>
     </row>
     <row r="42" spans="1:4" ht="30">
       <c r="A42" s="10" t="s">
@@ -5238,7 +5238,7 @@
       <c r="C42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="78"/>
+      <c r="D42" s="77"/>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="10" t="s">
@@ -5250,7 +5250,7 @@
       <c r="C43" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="78"/>
+      <c r="D43" s="77"/>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="10" t="s">
@@ -5262,7 +5262,7 @@
       <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="78"/>
+      <c r="D44" s="77"/>
     </row>
     <row r="52" spans="1:5" ht="27">
       <c r="A52" s="3" t="s">
@@ -5330,12 +5330,12 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="23">
-      <c r="A62" s="70" t="s">
+      <c r="A62" s="85" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="23">
-      <c r="A63" s="70" t="s">
+      <c r="A63" s="85" t="s">
         <v>868</v>
       </c>
       <c r="B63" s="42"/>
@@ -5632,10 +5632,10 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="D46" s="79"/>
+      <c r="D46" s="78"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="22" t="s">
@@ -5721,9 +5721,7 @@
   </sheetPr>
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="107" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>
@@ -5855,7 +5853,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="B16" s="83" t="s">
+      <c r="B16" s="82" t="s">
         <v>200</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -5869,7 +5867,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="84"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="58" t="s">
         <v>483</v>
       </c>
@@ -5881,7 +5879,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="82" t="s">
         <v>205</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -5895,7 +5893,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="84"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="26" t="s">
         <v>209</v>
       </c>
@@ -5907,7 +5905,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="82" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -5921,7 +5919,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="84"/>
+      <c r="B21" s="83"/>
       <c r="C21" s="26" t="s">
         <v>216</v>
       </c>
@@ -5961,7 +5959,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="82" t="s">
         <v>227</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -5975,7 +5973,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="85"/>
+      <c r="B25" s="84"/>
       <c r="C25" s="26" t="s">
         <v>229</v>
       </c>
@@ -5987,7 +5985,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="84"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="26" t="s">
         <v>232</v>
       </c>
@@ -6027,7 +6025,7 @@
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="80" t="s">
+      <c r="B35" s="79" t="s">
         <v>240</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -6041,7 +6039,7 @@
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="81"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="26" t="s">
         <v>243</v>
       </c>
@@ -6053,7 +6051,7 @@
       </c>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="81"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="26" t="s">
         <v>602</v>
       </c>
@@ -6065,7 +6063,7 @@
       </c>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="81"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="26" t="s">
         <v>248</v>
       </c>
@@ -6077,7 +6075,7 @@
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="81"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="26" t="s">
         <v>250</v>
       </c>
@@ -6089,7 +6087,7 @@
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="82"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="26" t="s">
         <v>252</v>
       </c>
@@ -6101,7 +6099,7 @@
       </c>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="79" t="s">
         <v>255</v>
       </c>
       <c r="C41" s="26" t="s">
@@ -6115,7 +6113,7 @@
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="81"/>
+      <c r="B42" s="80"/>
       <c r="C42" s="26" t="s">
         <v>259</v>
       </c>
@@ -6127,7 +6125,7 @@
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="81"/>
+      <c r="B43" s="80"/>
       <c r="C43" s="59" t="s">
         <v>604</v>
       </c>
@@ -6142,7 +6140,7 @@
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="81"/>
+      <c r="B44" s="80"/>
       <c r="C44" s="26" t="s">
         <v>603</v>
       </c>
@@ -6154,7 +6152,7 @@
       </c>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="81"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="26" t="s">
         <v>264</v>
       </c>
@@ -6169,7 +6167,7 @@
       </c>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="82"/>
+      <c r="B46" s="81"/>
       <c r="C46" s="26" t="s">
         <v>266</v>
       </c>
@@ -6182,10 +6180,10 @@
       <c r="L46" s="46"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="80" t="s">
+      <c r="B47" s="79" t="s">
         <v>268</v>
       </c>
-      <c r="C47" s="75" t="s">
+      <c r="C47" s="74" t="s">
         <v>269</v>
       </c>
       <c r="D47" s="26" t="s">
@@ -6199,8 +6197,8 @@
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="81"/>
-      <c r="C48" s="75" t="s">
+      <c r="B48" s="80"/>
+      <c r="C48" s="74" t="s">
         <v>272</v>
       </c>
       <c r="D48" s="26" t="s">
@@ -6212,8 +6210,8 @@
       <c r="L48" s="46"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="81"/>
-      <c r="C49" s="75" t="s">
+      <c r="B49" s="80"/>
+      <c r="C49" s="74" t="s">
         <v>275</v>
       </c>
       <c r="D49" s="26" t="s">
@@ -6227,8 +6225,8 @@
       </c>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="81"/>
-      <c r="C50" s="75" t="s">
+      <c r="B50" s="80"/>
+      <c r="C50" s="74" t="s">
         <v>278</v>
       </c>
       <c r="D50" s="26" t="s">
@@ -6240,8 +6238,8 @@
       <c r="L50" s="46"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="81"/>
-      <c r="C51" s="75" t="s">
+      <c r="B51" s="80"/>
+      <c r="C51" s="74" t="s">
         <v>281</v>
       </c>
       <c r="D51" s="26" t="s">
@@ -6255,8 +6253,8 @@
       </c>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="82"/>
-      <c r="C52" s="75" t="s">
+      <c r="B52" s="81"/>
+      <c r="C52" s="74" t="s">
         <v>284</v>
       </c>
       <c r="D52" s="26" t="s">
@@ -6267,7 +6265,7 @@
       </c>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="80" t="s">
+      <c r="B53" s="79" t="s">
         <v>287</v>
       </c>
       <c r="C53" s="26" t="s">
@@ -6281,7 +6279,7 @@
       </c>
     </row>
     <row r="54" spans="2:12">
-      <c r="B54" s="81"/>
+      <c r="B54" s="80"/>
       <c r="C54" s="26" t="s">
         <v>290</v>
       </c>
@@ -6293,7 +6291,7 @@
       </c>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="81"/>
+      <c r="B55" s="80"/>
       <c r="C55" s="26" t="s">
         <v>293</v>
       </c>
@@ -6305,7 +6303,7 @@
       </c>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="81"/>
+      <c r="B56" s="80"/>
       <c r="C56" s="26" t="s">
         <v>296</v>
       </c>
@@ -6317,7 +6315,7 @@
       </c>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="82"/>
+      <c r="B57" s="81"/>
       <c r="C57" s="26" t="s">
         <v>872</v>
       </c>
@@ -6329,7 +6327,7 @@
       </c>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="79" t="s">
         <v>301</v>
       </c>
       <c r="C58" s="26" t="s">
@@ -6343,7 +6341,7 @@
       </c>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="81"/>
+      <c r="B59" s="80"/>
       <c r="C59" s="26" t="s">
         <v>305</v>
       </c>
@@ -6355,7 +6353,7 @@
       </c>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="81"/>
+      <c r="B60" s="80"/>
       <c r="C60" s="26" t="s">
         <v>308</v>
       </c>
@@ -6367,7 +6365,7 @@
       </c>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="82"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="26" t="s">
         <v>311</v>
       </c>
@@ -7125,7 +7123,7 @@
       <c r="AH1" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="AQ1" s="74" t="s">
+      <c r="AQ1" s="73" t="s">
         <v>874</v>
       </c>
     </row>
@@ -7840,7 +7838,7 @@
       <c r="AH45" s="15" t="s">
         <v>628</v>
       </c>
-      <c r="AQ45" s="74" t="s">
+      <c r="AQ45" s="73" t="s">
         <v>895</v>
       </c>
     </row>
@@ -8416,7 +8414,7 @@
       <c r="AH89" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="AQ89" s="74" t="s">
+      <c r="AQ89" s="73" t="s">
         <v>916</v>
       </c>
     </row>
@@ -8750,7 +8748,7 @@
       <c r="AH133" s="15" t="s">
         <v>628</v>
       </c>
-      <c r="AQ133" s="74" t="s">
+      <c r="AQ133" s="73" t="s">
         <v>937</v>
       </c>
     </row>
@@ -9006,7 +9004,7 @@
       </c>
     </row>
     <row r="177" spans="43:43" ht="19">
-      <c r="AQ177" s="74" t="s">
+      <c r="AQ177" s="73" t="s">
         <v>958</v>
       </c>
     </row>
@@ -9122,8 +9120,8 @@
   </sheetPr>
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31" defaultRowHeight="16"/>
@@ -9163,7 +9161,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="20">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>275</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -9174,7 +9172,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="20">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="75" t="s">
         <v>278</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -9185,7 +9183,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="20">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="75" t="s">
         <v>281</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -9271,7 +9269,7 @@
       <c r="B17" s="52" t="s">
         <v>740</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="76" t="s">
         <v>706</v>
       </c>
       <c r="D17" s="52">
@@ -9313,7 +9311,7 @@
       <c r="B20" s="52" t="s">
         <v>742</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="76" t="s">
         <v>712</v>
       </c>
       <c r="D20" s="52">
@@ -9327,7 +9325,7 @@
       <c r="B21" s="52" t="s">
         <v>739</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="76" t="s">
         <v>714</v>
       </c>
       <c r="D21" s="52">
@@ -9341,7 +9339,7 @@
       <c r="B22" s="52" t="s">
         <v>743</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="76" t="s">
         <v>716</v>
       </c>
       <c r="D22" s="52">
@@ -9383,7 +9381,7 @@
       <c r="B25" s="52" t="s">
         <v>747</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="76" t="s">
         <v>721</v>
       </c>
       <c r="D25" s="52">
@@ -9714,7 +9712,7 @@
       <c r="E1" s="67" t="s">
         <v>756</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="70" t="s">
         <v>871</v>
       </c>
       <c r="G1" s="68" t="s">
@@ -9737,11 +9735,11 @@
       <c r="E2" s="63">
         <v>1</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="70" t="s">
         <v>290</v>
       </c>
       <c r="G2" s="69"/>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="71" t="s">
         <v>873</v>
       </c>
     </row>
@@ -9761,11 +9759,11 @@
       <c r="E3" s="63">
         <v>2</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="70" t="s">
         <v>293</v>
       </c>
       <c r="G3" s="64"/>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="71" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9781,11 +9779,11 @@
         <v>760</v>
       </c>
       <c r="E4" s="63"/>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="70" t="s">
         <v>296</v>
       </c>
       <c r="G4" s="64"/>
-      <c r="H4" s="72" t="s">
+      <c r="H4" s="71" t="s">
         <v>810</v>
       </c>
     </row>
@@ -9803,11 +9801,11 @@
       <c r="E5" s="63">
         <v>3</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="70" t="s">
         <v>872</v>
       </c>
       <c r="G5" s="64"/>
-      <c r="H5" s="73"/>
+      <c r="H5" s="72"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="63">
@@ -9826,7 +9824,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="69"/>
-      <c r="H6" s="73"/>
+      <c r="H6" s="72"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="63">

</xml_diff>